<commit_message>
Fix reference files: specify right styles for columns
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Styles/StyleIncludeQuotePrefix.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Styles/StyleIncludeQuotePrefix.xlsx
@@ -558,8 +558,8 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="2" width="3.960625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="10.340625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="12.730625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="10.340625" style="1" customWidth="1"/>
+    <x:col min="4" max="4" width="12.730625" style="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:4">

</xml_diff>

<commit_message>
Correctly load column-wide styles (#1135)
* Add a failing test for saving a column's number format

* Fix loading column styles

* Fix reference files: specify right styles for columns
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Styles/StyleIncludeQuotePrefix.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Styles/StyleIncludeQuotePrefix.xlsx
@@ -558,8 +558,8 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="2" width="3.960625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="10.340625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="12.730625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="10.340625" style="1" customWidth="1"/>
+    <x:col min="4" max="4" width="12.730625" style="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:4">

</xml_diff>